<commit_message>
Tratamento de pdfs ok no Alteryx
A R tool não pode lidar com o pacote tabulizer do R, mas consegui rodar os R scripts com a R Command.
</commit_message>
<xml_diff>
--- a/generalities_pdf.xlsx
+++ b/generalities_pdf.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">X__1</t>
   </si>
@@ -20,85 +20,73 @@
     <t xml:space="preserve">X__11</t>
   </si>
   <si>
-    <t xml:space="preserve">01 - GRIS (Gerenciamento de Risco): percentual sobre o valor da nota fiscal:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,30%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MinÃ­mo do GRIS em R$ por CT-e</t>
+    <t xml:space="preserve">gris_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gris_min</t>
   </si>
   <si>
     <t xml:space="preserve">isento</t>
   </si>
   <si>
-    <t xml:space="preserve">02 - PedÃ¡gio: em R$ por FraÃ§Ã£o de 100 Kg ou fraÃ§Ã£o</t>
+    <t xml:space="preserve">toll_value</t>
   </si>
   <si>
     <t xml:space="preserve">4,25</t>
   </si>
   <si>
-    <t xml:space="preserve">03 - Taxa de Despacho: para cada CT-e emitido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04 - TAS (Taxa de AdministraÃ§Ã£o SEFAZ): em R$ para cada CT-e emitido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CobranÃ§a em R$ para cada 100kg ou fraÃ§Ã£o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentual sobre valor da carga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 - Cubagem: mercadorias cujas densidades sejam superiores ao peso real serÃ£o CUBADAS na proporÃ§Ã£o de:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">280kg/m3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CobranÃ§a em percentual sobre o valor do frete praticado:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxa mÃ­nima TDE/TDA cobranÃ§a em R$:</t>
+    <t xml:space="preserve">delivery_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tas_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_fee_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_fee_fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cubic_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tda_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tda_min</t>
   </si>
   <si>
     <t xml:space="preserve">351,85</t>
   </si>
   <si>
-    <t xml:space="preserve">Taxa maxima TDE/TDA cobranÃ§a em R$:</t>
+    <t xml:space="preserve">tda_max</t>
   </si>
   <si>
     <t xml:space="preserve">882,43</t>
   </si>
   <si>
-    <t xml:space="preserve">agendamentos e nÃ£o estejam na relaÃ§Ã£o de TDE:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64,78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 - Entregas em Shopping: horÃ¡rio comercial: em R$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78,19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 - TRT (Taxa de RestriÃ§Ã£o de TrÃ¢nsito): em % sobre o valor do frete para cidades que apresentarem restriÃ§Ã£o para veiculos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxa mÃ­nima de TRT cobranÃ§a em R$:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICMS</t>
+    <t xml:space="preserve">trt_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trt_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icms_tax_enable</t>
   </si>
   <si>
     <t xml:space="preserve">true</t>
   </si>
   <si>
-    <t xml:space="preserve">ISS</t>
+    <t xml:space="preserve">iss_tax_enable</t>
   </si>
 </sst>
 </file>
@@ -531,47 +519,31 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>